<commit_message>
feat: add remote client and link to profile
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/vk.xlsx
+++ b/src/main/resources/excel/vk.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>0a5dbcdc-2e44-4579-a576-c93d5ee55485.png</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B719"/>
+  <dimension ref="A1:B720"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7626,6 +7629,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="720">
+      <c r="A720" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B720" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: add remote api config - take 1
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/vk.xlsx
+++ b/src/main/resources/excel/vk.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="2">
   <si>
     <t>image</t>
   </si>
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B720"/>
+  <dimension ref="A1:B745"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7637,6 +7637,206 @@
         <v>1</v>
       </c>
     </row>
+    <row r="721">
+      <c r="A721" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B721" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B722" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B723" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B724" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B725" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B726" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B727" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B728" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B729" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B730" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B731" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B732" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B733" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B734" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B735" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B736" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B737" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B738" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B739" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B740" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B741" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B742" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B743" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B744" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="n">
+        <v>126.0</v>
+      </c>
+      <c r="B745" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: add remote api config - take 1 (#11)
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/vk.xlsx
+++ b/src/main/resources/excel/vk.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="2">
   <si>
     <t>image</t>
   </si>
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B720"/>
+  <dimension ref="A1:B745"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7637,6 +7637,206 @@
         <v>1</v>
       </c>
     </row>
+    <row r="721">
+      <c r="A721" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B721" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B722" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B723" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B724" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B725" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B726" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B727" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B728" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B729" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B730" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B731" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B732" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B733" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B734" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B735" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B736" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B737" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B738" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B739" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B740" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B741" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B742" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B743" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B744" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="n">
+        <v>126.0</v>
+      </c>
+      <c r="B745" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: add remote api client prop
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/vk.xlsx
+++ b/src/main/resources/excel/vk.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="2">
   <si>
     <t>image</t>
   </si>
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B745"/>
+  <dimension ref="A1:B746"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7837,6 +7837,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="746">
+      <c r="A746" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B746" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: fix remote api client host
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/vk.xlsx
+++ b/src/main/resources/excel/vk.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="2">
   <si>
     <t>image</t>
   </si>
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B746"/>
+  <dimension ref="A1:B749"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7845,6 +7845,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="747">
+      <c r="A747" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B747" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B748" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B749" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>